<commit_message>
- La til variabel for stillingsandel - Justerte kva verdiar som blir tatt med i bruttolønnsvariabel - tar med fleire med redusert stilling - La til utskrift av stjerne(r) for signifikant endring, tok bort samanlagt N
</commit_message>
<xml_diff>
--- a/malfiler/Kandidat_2022_vars.xlsx
+++ b/malfiler/Kandidat_2022_vars.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hioa365-my.sharepoint.com/personal/kyrremat_oslomet_no/Documents/Dokumenter/statistikk/Studentsvar/malfiler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="603" documentId="8_{C41BFC7E-91D4-48D7-87E9-01433D7C7908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4822859-3013-49BE-92D3-9D731B7DB813}"/>
+  <xr:revisionPtr revIDLastSave="606" documentId="8_{C41BFC7E-91D4-48D7-87E9-01433D7C7908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03276ED8-E7BE-4309-B32F-D2613D888B28}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FA7D840D-9D53-4472-AAA2-57617C6B2F63}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="143">
   <si>
     <t>Variabel</t>
   </si>
@@ -455,6 +455,15 @@
   </si>
   <si>
     <t>Hvor lang tid tok det fra du fullførte utdanningen til du fikk tilbud om relevant jobb?</t>
+  </si>
+  <si>
+    <t>Brutto årslønn</t>
+  </si>
+  <si>
+    <t>brutto_arslonn_vasket</t>
+  </si>
+  <si>
+    <t>Vi har tatt bort svar som er under 300 000 og over 1 000 000 kr, og gjennomsnittet inkluderer bare de som oppgir å arbeide med det de er utdannet til.</t>
   </si>
 </sst>
 </file>
@@ -661,8 +670,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C5C1CF88-7443-457B-AC77-A0840E9FD512}" name="Table1" displayName="Table1" ref="A1:E38" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E38" xr:uid="{C5C1CF88-7443-457B-AC77-A0840E9FD512}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C5C1CF88-7443-457B-AC77-A0840E9FD512}" name="Table1" displayName="Table1" ref="A1:E39" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E39" xr:uid="{C5C1CF88-7443-457B-AC77-A0840E9FD512}"/>
   <tableColumns count="5">
     <tableColumn id="3" xr3:uid="{160CC1CB-F893-4D31-B90C-FCC9EC624563}" name="Spørsmålstekst" dataDxfId="4"/>
     <tableColumn id="4" xr3:uid="{26B093AC-730D-4DC7-8FEB-A32629DB4F75}" name="Variabel" dataDxfId="3"/>
@@ -971,10 +980,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11175198-0FD8-474C-BC80-0C4ED23782B1}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1547,6 +1556,23 @@
       </c>
       <c r="D38" s="2" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Tok bort "Annet" frå a5_hovedaktivitet, la til "Student" - Justerte variabel i malfil
</commit_message>
<xml_diff>
--- a/malfiler/Kandidat_2022_vars.xlsx
+++ b/malfiler/Kandidat_2022_vars.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hioa365-my.sharepoint.com/personal/kyrremat_oslomet_no/Documents/Dokumenter/statistikk/Studentsvar/malfiler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="606" documentId="8_{C41BFC7E-91D4-48D7-87E9-01433D7C7908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03276ED8-E7BE-4309-B32F-D2613D888B28}"/>
+  <xr:revisionPtr revIDLastSave="613" documentId="8_{C41BFC7E-91D4-48D7-87E9-01433D7C7908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17AE219B-7DA3-4C16-BF14-18B05F8604F4}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FA7D840D-9D53-4472-AAA2-57617C6B2F63}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="144">
   <si>
     <t>Variabel</t>
   </si>
@@ -445,9 +445,6 @@
     <t>fordeling_single</t>
   </si>
   <si>
-    <t>Før 2022 var svarene gitt med en firedelt skala, og vi har derfor ikke tatt med sammenligning av resultater.</t>
-  </si>
-  <si>
     <t>Spørsmålet var nytt i 2022.</t>
   </si>
   <si>
@@ -464,6 +461,12 @@
   </si>
   <si>
     <t>Vi har tatt bort svar som er under 300 000 og over 1 000 000 kr, og gjennomsnittet inkluderer bare de som oppgir å arbeide med det de er utdannet til.</t>
+  </si>
+  <si>
+    <t>I 2018 fikk ikke kandidatene oppfølgingsspørsmål om grunnen til redusert stilling, og vi har derfor ikke tatt med sammenligning av resultater.</t>
+  </si>
+  <si>
+    <t>Før 2022 var svarene gitt med en firedelt skala, vi har derfor ikke tatt med sammenligning av resultater.</t>
   </si>
 </sst>
 </file>
@@ -982,8 +985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11175198-0FD8-474C-BC80-0C4ED23782B1}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1136,10 +1139,13 @@
         <v>56</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>72</v>
+        <v>134</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>55</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1172,7 +1178,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>64</v>
@@ -1212,7 +1218,7 @@
         <v>69</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1229,7 +1235,7 @@
         <v>70</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1246,7 +1252,7 @@
         <v>104</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1263,7 +1269,7 @@
         <v>105</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1280,7 +1286,7 @@
         <v>123</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1297,7 +1303,7 @@
         <v>124</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1510,12 +1516,12 @@
         <v>121</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>44</v>
@@ -1527,7 +1533,7 @@
         <v>122</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1560,19 +1566,19 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>141</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>134</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- endra variabel for heltidsstilling for å få med personar med fleire stillingar - oppdaterte malfil
</commit_message>
<xml_diff>
--- a/malfiler/Kandidat_2022_vars.xlsx
+++ b/malfiler/Kandidat_2022_vars.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hioa365-my.sharepoint.com/personal/kyrremat_oslomet_no/Documents/Dokumenter/statistikk/Studentsvar/malfiler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="613" documentId="8_{C41BFC7E-91D4-48D7-87E9-01433D7C7908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17AE219B-7DA3-4C16-BF14-18B05F8604F4}"/>
+  <xr:revisionPtr revIDLastSave="616" documentId="8_{C41BFC7E-91D4-48D7-87E9-01433D7C7908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{050A270A-E263-4751-8F78-43374D90D8AB}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FA7D840D-9D53-4472-AAA2-57617C6B2F63}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="145">
   <si>
     <t>Variabel</t>
   </si>
@@ -196,277 +196,280 @@
     <t>mann</t>
   </si>
   <si>
+    <t>Andel heltid</t>
+  </si>
+  <si>
+    <t>Ufrivillig deltid</t>
+  </si>
+  <si>
+    <t>ufrivilligdeltid</t>
+  </si>
+  <si>
+    <t>Arkfanetittel</t>
+  </si>
+  <si>
+    <t>Hovedaktivitet</t>
+  </si>
+  <si>
+    <t>Studienivå nå</t>
+  </si>
+  <si>
+    <t>Arbeid samsvarer med utdanning</t>
+  </si>
+  <si>
+    <t>Forventning til arbeidsmarkedet</t>
+  </si>
+  <si>
+    <t>Sektor</t>
+  </si>
+  <si>
+    <t>Flere arbeidsgivere</t>
+  </si>
+  <si>
+    <t>dager_til_jobb</t>
+  </si>
+  <si>
+    <t>Dager til jobb</t>
+  </si>
+  <si>
+    <t>Hadde tilbud om jobb før fullført utdanning eller turnus</t>
+  </si>
+  <si>
+    <t>hadde_jobb_underveis</t>
+  </si>
+  <si>
+    <t>Hadde jobb underveis</t>
+  </si>
+  <si>
+    <t>Fornøyd med oppgaver (snitt)</t>
+  </si>
+  <si>
+    <t>Fornøyd med oppgaver (ford.)</t>
+  </si>
+  <si>
+    <t>fordeling</t>
+  </si>
+  <si>
+    <t>snitt_as_num</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Stilling påvirket av covid</t>
+  </si>
+  <si>
+    <t>Hovedbeskjeftigelse</t>
+  </si>
+  <si>
+    <t>Relevant arbeidsoppgaver snitt</t>
+  </si>
+  <si>
+    <t>Relevant arbeidsoppgaver ford</t>
+  </si>
+  <si>
+    <t>Dager til relevant jobb</t>
+  </si>
+  <si>
+    <t>Hadde relevant jobb før master</t>
+  </si>
+  <si>
+    <t>Nye oppgaver</t>
+  </si>
+  <si>
+    <t>Nødvendig for ansettelse</t>
+  </si>
+  <si>
+    <t>Sektortilhørighet</t>
+  </si>
+  <si>
+    <t>Arb.marked ift. forventning</t>
+  </si>
+  <si>
+    <t>Forberedt for arbeidsoppg</t>
+  </si>
+  <si>
+    <t>Forberedt for arbeidsoppg ford</t>
+  </si>
+  <si>
+    <t>Fornøyd m oppg - snitt</t>
+  </si>
+  <si>
+    <t>Fornøyd m oppg - fordeling</t>
+  </si>
+  <si>
+    <t>Læringsutb - alle</t>
+  </si>
+  <si>
+    <t>Læringsutb - teoretisk kunnskap</t>
+  </si>
+  <si>
+    <t>Læringsutb - metodiske ferdigh</t>
+  </si>
+  <si>
+    <t>Læringsutb - praktiske ferdigh</t>
+  </si>
+  <si>
+    <t>Læringsutb - analysere</t>
+  </si>
+  <si>
+    <t>Læringsutb - tilegne meg kunnsk</t>
+  </si>
+  <si>
+    <t>Læringsutb - kreativ innovativ</t>
+  </si>
+  <si>
+    <t>Læringsutb - formidle</t>
+  </si>
+  <si>
+    <t>Valgt samme utdanning - snitt</t>
+  </si>
+  <si>
+    <t>Valgt samme utd - fordeling</t>
+  </si>
+  <si>
+    <t>Samme lærested - snitt</t>
+  </si>
+  <si>
+    <t>Samme lærested - fordeling</t>
+  </si>
+  <si>
+    <t>Bachelorgrad fra OsloMet</t>
+  </si>
+  <si>
+    <t>Faner i 2020-rapport</t>
+  </si>
+  <si>
+    <t>Tatt med i 2022</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Forberedt for oppgaver (snitt)</t>
+  </si>
+  <si>
+    <t>Forberedt for oppgaver (ford.)</t>
+  </si>
+  <si>
+    <t>valgt_samme_institusjon</t>
+  </si>
+  <si>
+    <t>Valgt samme utdanning (snitt)</t>
+  </si>
+  <si>
+    <t>Valgt samme utd (ford.)</t>
+  </si>
+  <si>
+    <t>Valgt samme institusjon (snitt)</t>
+  </si>
+  <si>
+    <t>Valgt samme institusjon (ford.)</t>
+  </si>
+  <si>
+    <t>Aktiv i organisasjon</t>
+  </si>
+  <si>
+    <t>Aktiv i idrettslag</t>
+  </si>
+  <si>
+    <t>Aktiv i studentforening</t>
+  </si>
+  <si>
+    <t>Verv, klassetillitsvalgt</t>
+  </si>
+  <si>
+    <t>Verv, studentforening</t>
+  </si>
+  <si>
+    <t>Verv, studentrepresentant</t>
+  </si>
+  <si>
+    <t>Verv, studentparlamentet</t>
+  </si>
+  <si>
+    <t>Verv, ingen</t>
+  </si>
+  <si>
+    <t>Aktiv i ideell organisasjon</t>
+  </si>
+  <si>
+    <t>Aktiv i politisk organisasjon</t>
+  </si>
+  <si>
+    <t>Arbeidsgiver tilrettelegger VU</t>
+  </si>
+  <si>
+    <t>Arbeidsgiver finansierer VU</t>
+  </si>
+  <si>
+    <t>Tverrprof. kompetanse (snitt)</t>
+  </si>
+  <si>
+    <t>Tverrprof. kompetanse (ford.)</t>
+  </si>
+  <si>
+    <t>Kommentar</t>
+  </si>
+  <si>
+    <t>Kjønn, oppgitt som andel menn</t>
+  </si>
+  <si>
+    <t>I 2018 ble kandidatene spurt om de var ansatt i privat, statlig, kommunal eller frivillig sektor. Senere undersøkelser har hatt et alterniv for fylkeskommunal.</t>
+  </si>
+  <si>
+    <t>Hva er hovedgrunnen til at du ikke har full stilling?</t>
+  </si>
+  <si>
+    <t>grunn_redusert_stilling</t>
+  </si>
+  <si>
+    <t>Grunn redusert stilling</t>
+  </si>
+  <si>
+    <t>Hva er hovedgrunnen til at du ikke arbeider med det du er utdannet til?</t>
+  </si>
+  <si>
+    <t>grunn_annet_arbeid</t>
+  </si>
+  <si>
+    <t>Grunn annet arbeid</t>
+  </si>
+  <si>
+    <t>snitt_as_num_single</t>
+  </si>
+  <si>
+    <t>fordeling_single</t>
+  </si>
+  <si>
+    <t>Spørsmålet var nytt i 2022.</t>
+  </si>
+  <si>
+    <t>Pleier arbeidsgiveren din å finansiere videreutdanning?</t>
+  </si>
+  <si>
+    <t>Hvor lang tid tok det fra du fullførte utdanningen til du fikk tilbud om relevant jobb?</t>
+  </si>
+  <si>
+    <t>Brutto årslønn</t>
+  </si>
+  <si>
+    <t>brutto_arslonn_vasket</t>
+  </si>
+  <si>
+    <t>Vi har tatt bort svar som er under 300 000 og over 1 000 000 kr, og gjennomsnittet inkluderer bare de som oppgir å arbeide med det de er utdannet til.</t>
+  </si>
+  <si>
+    <t>I 2018 fikk ikke kandidatene oppfølgingsspørsmål om grunnen til redusert stilling, og vi har derfor ikke tatt med sammenligning av resultater.</t>
+  </si>
+  <si>
+    <t>Før 2022 var svarene gitt med en firedelt skala, vi har derfor ikke tatt med sammenligning av resultater.</t>
+  </si>
+  <si>
+    <t>Andel heltidsstilling</t>
+  </si>
+  <si>
     <t>heltidsstilling</t>
-  </si>
-  <si>
-    <t>Andel heltid</t>
-  </si>
-  <si>
-    <t>Ufrivillig deltid</t>
-  </si>
-  <si>
-    <t>ufrivilligdeltid</t>
-  </si>
-  <si>
-    <t>Arkfanetittel</t>
-  </si>
-  <si>
-    <t>Hovedaktivitet</t>
-  </si>
-  <si>
-    <t>Studienivå nå</t>
-  </si>
-  <si>
-    <t>Arbeid samsvarer med utdanning</t>
-  </si>
-  <si>
-    <t>Forventning til arbeidsmarkedet</t>
-  </si>
-  <si>
-    <t>Sektor</t>
-  </si>
-  <si>
-    <t>Flere arbeidsgivere</t>
-  </si>
-  <si>
-    <t>dager_til_jobb</t>
-  </si>
-  <si>
-    <t>Dager til jobb</t>
-  </si>
-  <si>
-    <t>Hadde tilbud om jobb før fullført utdanning eller turnus</t>
-  </si>
-  <si>
-    <t>hadde_jobb_underveis</t>
-  </si>
-  <si>
-    <t>Hadde jobb underveis</t>
-  </si>
-  <si>
-    <t>Fornøyd med oppgaver (snitt)</t>
-  </si>
-  <si>
-    <t>Fornøyd med oppgaver (ford.)</t>
-  </si>
-  <si>
-    <t>fordeling</t>
-  </si>
-  <si>
-    <t>snitt_as_num</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>Stilling påvirket av covid</t>
-  </si>
-  <si>
-    <t>Hovedbeskjeftigelse</t>
-  </si>
-  <si>
-    <t>Relevant arbeidsoppgaver snitt</t>
-  </si>
-  <si>
-    <t>Relevant arbeidsoppgaver ford</t>
-  </si>
-  <si>
-    <t>Dager til relevant jobb</t>
-  </si>
-  <si>
-    <t>Hadde relevant jobb før master</t>
-  </si>
-  <si>
-    <t>Nye oppgaver</t>
-  </si>
-  <si>
-    <t>Nødvendig for ansettelse</t>
-  </si>
-  <si>
-    <t>Sektortilhørighet</t>
-  </si>
-  <si>
-    <t>Arb.marked ift. forventning</t>
-  </si>
-  <si>
-    <t>Forberedt for arbeidsoppg</t>
-  </si>
-  <si>
-    <t>Forberedt for arbeidsoppg ford</t>
-  </si>
-  <si>
-    <t>Fornøyd m oppg - snitt</t>
-  </si>
-  <si>
-    <t>Fornøyd m oppg - fordeling</t>
-  </si>
-  <si>
-    <t>Læringsutb - alle</t>
-  </si>
-  <si>
-    <t>Læringsutb - teoretisk kunnskap</t>
-  </si>
-  <si>
-    <t>Læringsutb - metodiske ferdigh</t>
-  </si>
-  <si>
-    <t>Læringsutb - praktiske ferdigh</t>
-  </si>
-  <si>
-    <t>Læringsutb - analysere</t>
-  </si>
-  <si>
-    <t>Læringsutb - tilegne meg kunnsk</t>
-  </si>
-  <si>
-    <t>Læringsutb - kreativ innovativ</t>
-  </si>
-  <si>
-    <t>Læringsutb - formidle</t>
-  </si>
-  <si>
-    <t>Valgt samme utdanning - snitt</t>
-  </si>
-  <si>
-    <t>Valgt samme utd - fordeling</t>
-  </si>
-  <si>
-    <t>Samme lærested - snitt</t>
-  </si>
-  <si>
-    <t>Samme lærested - fordeling</t>
-  </si>
-  <si>
-    <t>Bachelorgrad fra OsloMet</t>
-  </si>
-  <si>
-    <t>Faner i 2020-rapport</t>
-  </si>
-  <si>
-    <t>Tatt med i 2022</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Forberedt for oppgaver (snitt)</t>
-  </si>
-  <si>
-    <t>Forberedt for oppgaver (ford.)</t>
-  </si>
-  <si>
-    <t>valgt_samme_institusjon</t>
-  </si>
-  <si>
-    <t>Valgt samme utdanning (snitt)</t>
-  </si>
-  <si>
-    <t>Valgt samme utd (ford.)</t>
-  </si>
-  <si>
-    <t>Valgt samme institusjon (snitt)</t>
-  </si>
-  <si>
-    <t>Valgt samme institusjon (ford.)</t>
-  </si>
-  <si>
-    <t>Aktiv i organisasjon</t>
-  </si>
-  <si>
-    <t>Aktiv i idrettslag</t>
-  </si>
-  <si>
-    <t>Aktiv i studentforening</t>
-  </si>
-  <si>
-    <t>Verv, klassetillitsvalgt</t>
-  </si>
-  <si>
-    <t>Verv, studentforening</t>
-  </si>
-  <si>
-    <t>Verv, studentrepresentant</t>
-  </si>
-  <si>
-    <t>Verv, studentparlamentet</t>
-  </si>
-  <si>
-    <t>Verv, ingen</t>
-  </si>
-  <si>
-    <t>Aktiv i ideell organisasjon</t>
-  </si>
-  <si>
-    <t>Aktiv i politisk organisasjon</t>
-  </si>
-  <si>
-    <t>Arbeidsgiver tilrettelegger VU</t>
-  </si>
-  <si>
-    <t>Arbeidsgiver finansierer VU</t>
-  </si>
-  <si>
-    <t>Tverrprof. kompetanse (snitt)</t>
-  </si>
-  <si>
-    <t>Tverrprof. kompetanse (ford.)</t>
-  </si>
-  <si>
-    <t>Kommentar</t>
-  </si>
-  <si>
-    <t>Kjønn, oppgitt som andel menn</t>
-  </si>
-  <si>
-    <t>I 2018 ble kandidatene spurt om de var ansatt i privat, statlig, kommunal eller frivillig sektor. Senere undersøkelser har hatt et alterniv for fylkeskommunal.</t>
-  </si>
-  <si>
-    <t>Hva er hovedgrunnen til at du ikke har full stilling?</t>
-  </si>
-  <si>
-    <t>grunn_redusert_stilling</t>
-  </si>
-  <si>
-    <t>Grunn redusert stilling</t>
-  </si>
-  <si>
-    <t>Hva er hovedgrunnen til at du ikke arbeider med det du er utdannet til?</t>
-  </si>
-  <si>
-    <t>grunn_annet_arbeid</t>
-  </si>
-  <si>
-    <t>Grunn annet arbeid</t>
-  </si>
-  <si>
-    <t>snitt_as_num_single</t>
-  </si>
-  <si>
-    <t>fordeling_single</t>
-  </si>
-  <si>
-    <t>Spørsmålet var nytt i 2022.</t>
-  </si>
-  <si>
-    <t>Pleier arbeidsgiveren din å finansiere videreutdanning?</t>
-  </si>
-  <si>
-    <t>Hvor lang tid tok det fra du fullførte utdanningen til du fikk tilbud om relevant jobb?</t>
-  </si>
-  <si>
-    <t>Brutto årslønn</t>
-  </si>
-  <si>
-    <t>brutto_arslonn_vasket</t>
-  </si>
-  <si>
-    <t>Vi har tatt bort svar som er under 300 000 og over 1 000 000 kr, og gjennomsnittet inkluderer bare de som oppgir å arbeide med det de er utdannet til.</t>
-  </si>
-  <si>
-    <t>I 2018 fikk ikke kandidatene oppfølgingsspørsmål om grunnen til redusert stilling, og vi har derfor ikke tatt med sammenligning av resultater.</t>
-  </si>
-  <si>
-    <t>Før 2022 var svarene gitt med en firedelt skala, vi har derfor ikke tatt med sammenligning av resultater.</t>
   </si>
 </sst>
 </file>
@@ -510,7 +513,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -519,6 +522,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -985,8 +991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11175198-0FD8-474C-BC80-0C4ED23782B1}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1010,10 +1016,10 @@
         <v>45</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1024,10 +1030,10 @@
         <v>46</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1038,10 +1044,10 @@
         <v>24</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1052,24 +1058,24 @@
         <v>25</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1080,10 +1086,10 @@
         <v>26</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1094,13 +1100,13 @@
         <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1111,7 +1117,7 @@
         <v>48</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>47</v>
@@ -1119,47 +1125,47 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="C10" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1170,38 +1176,38 @@
         <v>28</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1212,13 +1218,13 @@
         <v>29</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1229,13 +1235,13 @@
         <v>29</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1246,13 +1252,13 @@
         <v>30</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1263,13 +1269,13 @@
         <v>30</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1280,13 +1286,13 @@
         <v>31</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1297,13 +1303,13 @@
         <v>31</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1314,10 +1320,10 @@
         <v>32</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1328,10 +1334,10 @@
         <v>32</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1339,13 +1345,13 @@
         <v>12</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1353,13 +1359,13 @@
         <v>12</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D24" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1370,10 +1376,10 @@
         <v>33</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1384,10 +1390,10 @@
         <v>34</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1398,10 +1404,10 @@
         <v>35</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1412,10 +1418,10 @@
         <v>36</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1426,10 +1432,10 @@
         <v>37</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1440,10 +1446,10 @@
         <v>38</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1454,10 +1460,10 @@
         <v>39</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1468,10 +1474,10 @@
         <v>40</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1482,10 +1488,10 @@
         <v>41</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1496,10 +1502,10 @@
         <v>42</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1510,41 +1516,41 @@
         <v>43</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>52</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>49</v>
@@ -1558,7 +1564,7 @@
         <v>51</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>50</v>
@@ -1566,19 +1572,19 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="C39" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1611,82 +1617,82 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
         <v>101</v>
-      </c>
-      <c r="B1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1694,128 +1700,128 @@
         <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
- Retta opp omkoding basert på fritekstsvar - La til variabel for deltidsstilling - Rydding - Justerte maldokument for å ta med variabel for deltidsstilling
</commit_message>
<xml_diff>
--- a/malfiler/Kandidat_2022_vars.xlsx
+++ b/malfiler/Kandidat_2022_vars.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hioa365-my.sharepoint.com/personal/kyrremat_oslomet_no/Documents/Dokumenter/statistikk/Studentsvar/malfiler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="616" documentId="8_{C41BFC7E-91D4-48D7-87E9-01433D7C7908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{050A270A-E263-4751-8F78-43374D90D8AB}"/>
+  <xr:revisionPtr revIDLastSave="622" documentId="8_{C41BFC7E-91D4-48D7-87E9-01433D7C7908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FBEC6B38-6E9E-4245-97D8-8D8A33C64201}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FA7D840D-9D53-4472-AAA2-57617C6B2F63}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="148">
   <si>
     <t>Variabel</t>
   </si>
@@ -415,9 +415,6 @@
     <t>Kjønn, oppgitt som andel menn</t>
   </si>
   <si>
-    <t>I 2018 ble kandidatene spurt om de var ansatt i privat, statlig, kommunal eller frivillig sektor. Senere undersøkelser har hatt et alterniv for fylkeskommunal.</t>
-  </si>
-  <si>
     <t>Hva er hovedgrunnen til at du ikke har full stilling?</t>
   </si>
   <si>
@@ -470,6 +467,18 @@
   </si>
   <si>
     <t>heltidsstilling</t>
+  </si>
+  <si>
+    <t>I 2018 ble kandidatene spurt om de var ansatt i privat, statlig, kommunal eller frivillig sektor. Senere undersøkelser har hatt et alternativ for fylkeskommunal.</t>
+  </si>
+  <si>
+    <t>Andel deltid</t>
+  </si>
+  <si>
+    <t>deltidsstilling</t>
+  </si>
+  <si>
+    <t>Andel deltidsstilling</t>
   </si>
 </sst>
 </file>
@@ -679,8 +688,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C5C1CF88-7443-457B-AC77-A0840E9FD512}" name="Table1" displayName="Table1" ref="A1:E39" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E39" xr:uid="{C5C1CF88-7443-457B-AC77-A0840E9FD512}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C5C1CF88-7443-457B-AC77-A0840E9FD512}" name="Table1" displayName="Table1" ref="A1:E40" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E40" xr:uid="{C5C1CF88-7443-457B-AC77-A0840E9FD512}"/>
   <tableColumns count="5">
     <tableColumn id="3" xr3:uid="{160CC1CB-F893-4D31-B90C-FCC9EC624563}" name="Spørsmålstekst" dataDxfId="4"/>
     <tableColumn id="4" xr3:uid="{26B093AC-730D-4DC7-8FEB-A32629DB4F75}" name="Variabel" dataDxfId="3"/>
@@ -989,7 +998,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11175198-0FD8-474C-BC80-0C4ED23782B1}">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
@@ -1066,16 +1075,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>131</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>70</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1106,7 +1115,7 @@
         <v>61</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>126</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1125,106 +1134,103 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>53</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>55</v>
+        <v>142</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>143</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>133</v>
+        <v>71</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>141</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>127</v>
+        <v>54</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>128</v>
+        <v>55</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>70</v>
+        <v>132</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>129</v>
+        <v>54</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="C13" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D14" s="2" t="s">
+      <c r="C15" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1235,30 +1241,30 @@
         <v>29</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>133</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>103</v>
+        <v>69</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1269,30 +1275,30 @@
         <v>30</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>133</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1303,27 +1309,30 @@
         <v>31</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D21" t="s">
-        <v>106</v>
+        <v>133</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1334,24 +1343,24 @@
         <v>32</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>105</v>
+        <v>32</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1362,229 +1371,243 @@
         <v>105</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>33</v>
+        <v>105</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>110</v>
+        <v>70</v>
+      </c>
+      <c r="D25" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>133</v>
+        <v>71</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>136</v>
+        <v>23</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>71</v>
+        <v>132</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>49</v>
+        <v>121</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>50</v>
+        <v>125</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="C40" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Justerte rekoding av nokre variablar - La til avrunding for lønnsvariabel - Justerte malfiler
</commit_message>
<xml_diff>
--- a/malfiler/Kandidat_2022_vars.xlsx
+++ b/malfiler/Kandidat_2022_vars.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hioa365-my.sharepoint.com/personal/kyrremat_oslomet_no/Documents/Dokumenter/statistikk/Studentsvar/malfiler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="622" documentId="8_{C41BFC7E-91D4-48D7-87E9-01433D7C7908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FBEC6B38-6E9E-4245-97D8-8D8A33C64201}"/>
+  <xr:revisionPtr revIDLastSave="626" documentId="8_{C41BFC7E-91D4-48D7-87E9-01433D7C7908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{19B068DE-91B0-44EA-84EB-F7D681B93130}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FA7D840D-9D53-4472-AAA2-57617C6B2F63}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="121">
   <si>
     <t>Variabel</t>
   </si>
@@ -79,33 +79,6 @@
     <t>Var du aktiv i en organisasjon, forening eller lag under studietiden?</t>
   </si>
   <si>
-    <t>Hva slags organisasjon, forening eller lag var du aktiv i? [Idrettslag]</t>
-  </si>
-  <si>
-    <t>Hva slags organisasjon, forening eller lag var du aktiv i? [Studentforening]</t>
-  </si>
-  <si>
-    <t>Hva slags organisasjon, forening eller lag var du aktiv i? [Ideell organisasjon / interesseorganisasjon ]</t>
-  </si>
-  <si>
-    <t>Hva slags organisasjon, forening eller lag var du aktiv i? [Politisk parti]</t>
-  </si>
-  <si>
-    <t>Hadde du noen av de følgende vervene mens du var student? [Klassetillitsvalgt]</t>
-  </si>
-  <si>
-    <t>Hadde du noen av de følgende vervene mens du var student? [Styremedlem eller leder i studentforening]</t>
-  </si>
-  <si>
-    <t>Hadde du noen av de følgende vervene mens du var student? [Studentrepresentant i styre, råd eller utvalg ved OsloMet (tidligere HiOA)]</t>
-  </si>
-  <si>
-    <t>Hadde du noen av de følgende vervene mens du var student? [Medlem i studentparlamentet]</t>
-  </si>
-  <si>
-    <t>Hadde du noen av de følgende vervene mens du var student? [Nei, ingen av disse vervene]</t>
-  </si>
-  <si>
     <t>Legger arbeidsgiveren din tilrette for at du kan ta studiepoenggivende videreutdanning dersom du ønsker det?</t>
   </si>
   <si>
@@ -139,33 +112,6 @@
     <t>aktiv_organisasjon</t>
   </si>
   <si>
-    <t>aktiv_idrettslag</t>
-  </si>
-  <si>
-    <t>aktiv_studentforening</t>
-  </si>
-  <si>
-    <t>aktiv_ideell</t>
-  </si>
-  <si>
-    <t>aktiv_politisk</t>
-  </si>
-  <si>
-    <t>verv_klassetillitsvalgt</t>
-  </si>
-  <si>
-    <t>verv_studentforening</t>
-  </si>
-  <si>
-    <t>verv_studentrepresentant</t>
-  </si>
-  <si>
-    <t>verv_studentparlamentet</t>
-  </si>
-  <si>
-    <t>verv_ingen</t>
-  </si>
-  <si>
     <t>arbeidsgiver_tilrettelegger_videreutdanning</t>
   </si>
   <si>
@@ -368,33 +314,6 @@
   </si>
   <si>
     <t>Aktiv i organisasjon</t>
-  </si>
-  <si>
-    <t>Aktiv i idrettslag</t>
-  </si>
-  <si>
-    <t>Aktiv i studentforening</t>
-  </si>
-  <si>
-    <t>Verv, klassetillitsvalgt</t>
-  </si>
-  <si>
-    <t>Verv, studentforening</t>
-  </si>
-  <si>
-    <t>Verv, studentrepresentant</t>
-  </si>
-  <si>
-    <t>Verv, studentparlamentet</t>
-  </si>
-  <si>
-    <t>Verv, ingen</t>
-  </si>
-  <si>
-    <t>Aktiv i ideell organisasjon</t>
-  </si>
-  <si>
-    <t>Aktiv i politisk organisasjon</t>
   </si>
   <si>
     <t>Arbeidsgiver tilrettelegger VU</t>
@@ -688,8 +607,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C5C1CF88-7443-457B-AC77-A0840E9FD512}" name="Table1" displayName="Table1" ref="A1:E40" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E40" xr:uid="{C5C1CF88-7443-457B-AC77-A0840E9FD512}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C5C1CF88-7443-457B-AC77-A0840E9FD512}" name="Table1" displayName="Table1" ref="A1:E31" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E31" xr:uid="{C5C1CF88-7443-457B-AC77-A0840E9FD512}"/>
   <tableColumns count="5">
     <tableColumn id="3" xr3:uid="{160CC1CB-F893-4D31-B90C-FCC9EC624563}" name="Spørsmålstekst" dataDxfId="4"/>
     <tableColumn id="4" xr3:uid="{26B093AC-730D-4DC7-8FEB-A32629DB4F75}" name="Variabel" dataDxfId="3"/>
@@ -998,10 +917,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11175198-0FD8-474C-BC80-0C4ED23782B1}">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1022,13 +941,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1036,13 +955,13 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1050,13 +969,13 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1064,27 +983,27 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>130</v>
+        <v>103</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>131</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1092,13 +1011,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1106,89 +1025,89 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>146</v>
+        <v>119</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>145</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>142</v>
+        <v>115</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>132</v>
+        <v>105</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>140</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>126</v>
+        <v>99</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>127</v>
+        <v>100</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>128</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1196,41 +1115,41 @@
         <v>7</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>136</v>
+        <v>109</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1238,16 +1157,16 @@
         <v>8</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>132</v>
+        <v>105</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>141</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1255,16 +1174,16 @@
         <v>8</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>133</v>
+        <v>106</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>141</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1272,16 +1191,16 @@
         <v>9</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>132</v>
+        <v>105</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>141</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1289,16 +1208,16 @@
         <v>9</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>133</v>
+        <v>106</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>141</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1306,16 +1225,16 @@
         <v>10</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>132</v>
+        <v>105</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>122</v>
+        <v>95</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>134</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1323,16 +1242,16 @@
         <v>10</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>133</v>
+        <v>106</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>123</v>
+        <v>96</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>134</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1340,13 +1259,13 @@
         <v>11</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="D22" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1354,13 +1273,13 @@
         <v>11</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="D23" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1368,13 +1287,13 @@
         <v>12</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="D24" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1382,13 +1301,13 @@
         <v>12</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="D25" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1396,13 +1315,13 @@
         <v>13</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1410,204 +1329,78 @@
         <v>14</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>111</v>
+        <v>93</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>15</v>
+        <v>108</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>112</v>
+        <v>94</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>16</v>
+        <v>98</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>118</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>119</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>18</v>
+        <v>110</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>38</v>
+        <v>111</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>139</v>
+        <v>110</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1640,221 +1433,221 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="B1" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="B5" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="B8" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="B9" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
         <v>54</v>
-      </c>
-      <c r="B13" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="B14" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="B15" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="B16" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="B17" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- La til variabel får ikkje relevant arbeid innan 6 månader - Rydda i faktor - Justert malfiler
</commit_message>
<xml_diff>
--- a/malfiler/Kandidat_2022_vars.xlsx
+++ b/malfiler/Kandidat_2022_vars.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hioa365-my.sharepoint.com/personal/kyrremat_oslomet_no/Documents/Dokumenter/statistikk/Studentsvar/malfiler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="626" documentId="8_{C41BFC7E-91D4-48D7-87E9-01433D7C7908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{19B068DE-91B0-44EA-84EB-F7D681B93130}"/>
+  <xr:revisionPtr revIDLastSave="630" documentId="8_{C41BFC7E-91D4-48D7-87E9-01433D7C7908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F36ACEB-44E6-4AF0-A989-86F14DC1156A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FA7D840D-9D53-4472-AAA2-57617C6B2F63}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="118">
   <si>
     <t>Variabel</t>
   </si>
@@ -76,9 +76,6 @@
     <t>Tenk deg at det hadde vært mulig å gjøre om igjen det valget du foretok da du begynte på studiet. Hvor sannsynlig er det at du da ville ha valgt ... [samme lærested?]</t>
   </si>
   <si>
-    <t>Var du aktiv i en organisasjon, forening eller lag under studietiden?</t>
-  </si>
-  <si>
     <t>Legger arbeidsgiveren din tilrette for at du kan ta studiepoenggivende videreutdanning dersom du ønsker det?</t>
   </si>
   <si>
@@ -109,9 +106,6 @@
     <t>valgt_samme_utdanning</t>
   </si>
   <si>
-    <t>aktiv_organisasjon</t>
-  </si>
-  <si>
     <t>arbeidsgiver_tilrettelegger_videreutdanning</t>
   </si>
   <si>
@@ -172,12 +166,6 @@
     <t>Flere arbeidsgivere</t>
   </si>
   <si>
-    <t>dager_til_jobb</t>
-  </si>
-  <si>
-    <t>Dager til jobb</t>
-  </si>
-  <si>
     <t>Hadde tilbud om jobb før fullført utdanning eller turnus</t>
   </si>
   <si>
@@ -313,9 +301,6 @@
     <t>Valgt samme institusjon (ford.)</t>
   </si>
   <si>
-    <t>Aktiv i organisasjon</t>
-  </si>
-  <si>
     <t>Arbeidsgiver tilrettelegger VU</t>
   </si>
   <si>
@@ -364,9 +349,6 @@
     <t>Pleier arbeidsgiveren din å finansiere videreutdanning?</t>
   </si>
   <si>
-    <t>Hvor lang tid tok det fra du fullførte utdanningen til du fikk tilbud om relevant jobb?</t>
-  </si>
-  <si>
     <t>Brutto årslønn</t>
   </si>
   <si>
@@ -398,6 +380,15 @@
   </si>
   <si>
     <t>Andel deltidsstilling</t>
+  </si>
+  <si>
+    <t>Tok det mer enn 6 måneder å få relevant arbeid?</t>
+  </si>
+  <si>
+    <t>lang_tid_til_relevant_arbeid</t>
+  </si>
+  <si>
+    <t>Lang tid til relevant arbeid</t>
   </si>
 </sst>
 </file>
@@ -441,7 +432,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -453,6 +444,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -607,8 +601,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C5C1CF88-7443-457B-AC77-A0840E9FD512}" name="Table1" displayName="Table1" ref="A1:E31" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E31" xr:uid="{C5C1CF88-7443-457B-AC77-A0840E9FD512}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C5C1CF88-7443-457B-AC77-A0840E9FD512}" name="Table1" displayName="Table1" ref="A1:E30" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E30" xr:uid="{C5C1CF88-7443-457B-AC77-A0840E9FD512}"/>
   <tableColumns count="5">
     <tableColumn id="3" xr3:uid="{160CC1CB-F893-4D31-B90C-FCC9EC624563}" name="Spørsmålstekst" dataDxfId="4"/>
     <tableColumn id="4" xr3:uid="{26B093AC-730D-4DC7-8FEB-A32629DB4F75}" name="Variabel" dataDxfId="3"/>
@@ -917,10 +911,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11175198-0FD8-474C-BC80-0C4ED23782B1}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="A26" sqref="A26:D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,13 +935,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -955,13 +949,13 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -969,13 +963,13 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -983,27 +977,27 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1011,13 +1005,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1025,89 +1019,89 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1115,41 +1109,41 @@
         <v>7</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>109</v>
+        <v>43</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>49</v>
+      <c r="A15" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1157,16 +1151,16 @@
         <v>8</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1174,16 +1168,16 @@
         <v>8</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1191,16 +1185,16 @@
         <v>9</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1208,16 +1202,16 @@
         <v>9</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1225,16 +1219,16 @@
         <v>10</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1242,16 +1236,16 @@
         <v>10</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1259,13 +1253,13 @@
         <v>11</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D22" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1273,13 +1267,13 @@
         <v>11</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D23" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1287,13 +1281,13 @@
         <v>12</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D24" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1301,13 +1295,13 @@
         <v>12</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" t="s">
         <v>87</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D25" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1315,92 +1309,78 @@
         <v>13</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>53</v>
+        <v>100</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>14</v>
+        <v>103</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>105</v>
+        <v>49</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>107</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>98</v>
+        <v>30</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>32</v>
+        <v>104</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>33</v>
+        <v>105</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>53</v>
+        <v>100</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>112</v>
+        <v>104</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1433,221 +1413,221 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B8" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B9" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Meir generisk koding av faktor - Fjerna utgått kode og justert kommentarar
</commit_message>
<xml_diff>
--- a/malfiler/Kandidat_2022_vars.xlsx
+++ b/malfiler/Kandidat_2022_vars.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hioa365-my.sharepoint.com/personal/kyrremat_oslomet_no/Documents/Dokumenter/statistikk/Studentsvar/malfiler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="630" documentId="8_{C41BFC7E-91D4-48D7-87E9-01433D7C7908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F36ACEB-44E6-4AF0-A989-86F14DC1156A}"/>
+  <xr:revisionPtr revIDLastSave="641" documentId="8_{C41BFC7E-91D4-48D7-87E9-01433D7C7908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59746181-757C-4F70-A3D0-FCA4DBCE2494}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FA7D840D-9D53-4472-AAA2-57617C6B2F63}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="116">
   <si>
     <t>Variabel</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Spørsmålstekst</t>
   </si>
   <si>
-    <t>Hva er din hovedaktivitet?  Velg den aktiviteten du bruker mest tid på. Se bort fra om du for tiden er sykemeldt eller i permisjon.</t>
-  </si>
-  <si>
     <t>På hvilket nivå studerer du nå?</t>
   </si>
   <si>
@@ -61,21 +58,6 @@
     <t>Er du ansatt hos mer enn én arbeidsgiver?</t>
   </si>
   <si>
-    <t>Hvor enig er du i følgende utsagn? [Jeg er godt fornøyd med oppgaver og ansvar i min nåværende jobb.]</t>
-  </si>
-  <si>
-    <t>Hvor enig er du i følgende utsagn? [Utdanningen forberedte meg godt for oppgaver og ansvar i min nåværende jobb.]</t>
-  </si>
-  <si>
-    <t>Hvor enig er du i følgende utsagn? [Utdanningen ga meg kompetanse i å samarbeide med andre yrkesgrupper (tverrprofesjonelt samarbeid)]</t>
-  </si>
-  <si>
-    <t>Tenk deg at det hadde vært mulig å gjøre om igjen det valget du foretok da du begynte på studiet. Hvor sannsynlig er det at du da ville ha valgt ... [samme type utdanning?]</t>
-  </si>
-  <si>
-    <t>Tenk deg at det hadde vært mulig å gjøre om igjen det valget du foretok da du begynte på studiet. Hvor sannsynlig er det at du da ville ha valgt ... [samme lærested?]</t>
-  </si>
-  <si>
     <t>Legger arbeidsgiveren din tilrette for at du kan ta studiepoenggivende videreutdanning dersom du ønsker det?</t>
   </si>
   <si>
@@ -358,18 +340,9 @@
     <t>Vi har tatt bort svar som er under 300 000 og over 1 000 000 kr, og gjennomsnittet inkluderer bare de som oppgir å arbeide med det de er utdannet til.</t>
   </si>
   <si>
-    <t>I 2018 fikk ikke kandidatene oppfølgingsspørsmål om grunnen til redusert stilling, og vi har derfor ikke tatt med sammenligning av resultater.</t>
-  </si>
-  <si>
     <t>Før 2022 var svarene gitt med en firedelt skala, vi har derfor ikke tatt med sammenligning av resultater.</t>
   </si>
   <si>
-    <t>Andel heltidsstilling</t>
-  </si>
-  <si>
-    <t>heltidsstilling</t>
-  </si>
-  <si>
     <t>I 2018 ble kandidatene spurt om de var ansatt i privat, statlig, kommunal eller frivillig sektor. Senere undersøkelser har hatt et alternativ for fylkeskommunal.</t>
   </si>
   <si>
@@ -389,6 +362,27 @@
   </si>
   <si>
     <t>Lang tid til relevant arbeid</t>
+  </si>
+  <si>
+    <t>Utdanningen ga meg kompetanse i å samarbeide med andre yrkesgrupper (tverrprofesjonelt samarbeid)</t>
+  </si>
+  <si>
+    <t>Hvor sannsynlig er det at du ville ha valgt samme type utdanning?</t>
+  </si>
+  <si>
+    <t>Hvor sannsynlig er det at du ville ha valgt samme lærested?</t>
+  </si>
+  <si>
+    <t>Andel av de som arbeider deltid og som ønsker full stilling. I 2018 fikk ikke kandidatene oppfølgingsspørsmål om grunnen til redusert stilling, og vi har derfor ikke tatt med sammenligning av resultater.</t>
+  </si>
+  <si>
+    <t>Jeg er godt fornøyd med oppgaver og ansvar i min nåværende jobb</t>
+  </si>
+  <si>
+    <t>Utdanningen forberedte meg godt for oppgaver og ansvar i min nåværende jobb</t>
+  </si>
+  <si>
+    <t>Hovedaktivitet 1–3 år etter fullført utdanning</t>
   </si>
 </sst>
 </file>
@@ -601,8 +595,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C5C1CF88-7443-457B-AC77-A0840E9FD512}" name="Table1" displayName="Table1" ref="A1:E30" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E30" xr:uid="{C5C1CF88-7443-457B-AC77-A0840E9FD512}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C5C1CF88-7443-457B-AC77-A0840E9FD512}" name="Table1" displayName="Table1" ref="A1:E29" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E29" xr:uid="{C5C1CF88-7443-457B-AC77-A0840E9FD512}"/>
   <tableColumns count="5">
     <tableColumn id="3" xr3:uid="{160CC1CB-F893-4D31-B90C-FCC9EC624563}" name="Spørsmålstekst" dataDxfId="4"/>
     <tableColumn id="4" xr3:uid="{26B093AC-730D-4DC7-8FEB-A32629DB4F75}" name="Variabel" dataDxfId="3"/>
@@ -911,10 +905,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11175198-0FD8-474C-BC80-0C4ED23782B1}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:D26"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -935,452 +929,438 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>115</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>110</v>
+        <v>28</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>49</v>
+        <v>94</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>34</v>
+        <v>88</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>35</v>
+        <v>89</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C12" s="2" t="s">
+      <c r="D15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>8</v>
+        <v>113</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>8</v>
+        <v>114</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>9</v>
+        <v>114</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>9</v>
+        <v>109</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>10</v>
+        <v>109</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>10</v>
+        <v>110</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>102</v>
+        <v>43</v>
+      </c>
+      <c r="D21" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>11</v>
+        <v>110</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D22" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>22</v>
+        <v>77</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D23" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>12</v>
+        <v>111</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D24" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>83</v>
+        <v>17</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D25" t="s">
-        <v>87</v>
+        <v>94</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>13</v>
+        <v>97</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>100</v>
+        <v>43</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>102</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>93</v>
+        <v>24</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>30</v>
+        <v>98</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>31</v>
+        <v>99</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>49</v>
+        <v>94</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C30" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1413,221 +1393,221 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Justerte fakultetsnamn - Avgrensa to variablar (fornoyd_oppgaver, forberedt_oppgaver) til å berre gjelde dei med relevant arbeid - La til faktorvariabel for arbeider i Oslo, Viken eller anna - Sortert utskrift i baklengs rekkefølgje for å vise rett veg i diagram - Oppdaterte malfiler
</commit_message>
<xml_diff>
--- a/malfiler/Kandidat_2022_vars.xlsx
+++ b/malfiler/Kandidat_2022_vars.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hioa365-my.sharepoint.com/personal/kyrremat_oslomet_no/Documents/Dokumenter/statistikk/Studentsvar/malfiler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="641" documentId="8_{C41BFC7E-91D4-48D7-87E9-01433D7C7908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59746181-757C-4F70-A3D0-FCA4DBCE2494}"/>
+  <xr:revisionPtr revIDLastSave="649" documentId="8_{C41BFC7E-91D4-48D7-87E9-01433D7C7908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{062E9527-C5A7-4CD0-B2B8-63C906E06BA0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FA7D840D-9D53-4472-AAA2-57617C6B2F63}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="118">
   <si>
     <t>Variabel</t>
   </si>
@@ -103,9 +103,6 @@
     <t>Jobber i Oslo</t>
   </si>
   <si>
-    <t>oslo</t>
-  </si>
-  <si>
     <t>Kjønn</t>
   </si>
   <si>
@@ -383,6 +380,15 @@
   </si>
   <si>
     <t>Hovedaktivitet 1–3 år etter fullført utdanning</t>
+  </si>
+  <si>
+    <t>Hvor er arbeidsstedet ditt?</t>
+  </si>
+  <si>
+    <t>oslo_viken_annet</t>
+  </si>
+  <si>
+    <t>Arbeidssted</t>
   </si>
 </sst>
 </file>
@@ -908,7 +914,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A8" sqref="A8:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -932,24 +938,24 @@
         <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -960,10 +966,10 @@
         <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -974,24 +980,24 @@
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1002,10 +1008,10 @@
         <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1016,72 +1022,72 @@
         <v>11</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>21</v>
+        <v>115</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>22</v>
+        <v>116</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>21</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="C10" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1092,196 +1098,196 @@
         <v>12</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="C14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>107</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1292,75 +1298,75 @@
         <v>17</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="C28" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="C29" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1393,82 +1399,82 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" t="s">
         <v>72</v>
-      </c>
-      <c r="B1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1476,138 +1482,138 @@
         <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>